<commit_message>
Add file for questions.
</commit_message>
<xml_diff>
--- a/AngularComplete/Question.xlsx
+++ b/AngularComplete/Question.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Projects\AngularCompleteGuide\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Projects\AngularCompleteGuide\AngularComplete\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{24DC30AF-7FA9-41ED-A9D2-CC5BAC1D1066}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FC376CD-FC03-4F37-AF67-8CA29BE38F5E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11565" xr2:uid="{0E520718-C840-4664-8426-238CA800352E}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11565" activeTab="1" xr2:uid="{0E520718-C840-4664-8426-238CA800352E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,25 +32,148 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="29">
   <si>
     <t>Question</t>
   </si>
   <si>
     <t>Answers</t>
+  </si>
+  <si>
+    <t>Difference Between ASP.NET and ASP MVC</t>
+  </si>
+  <si>
+    <t>ASP.Net Web Form</t>
+  </si>
+  <si>
+    <t>ASP.Net MVC</t>
+  </si>
+  <si>
+    <t>ASP.NET Web Forms uses Page controller pattern approach for rendering layout. In this approach, every page has it’s own controller i.e. code-behind file that processes the request.</t>
+  </si>
+  <si>
+    <t>ASP.NET MVC uses Front Controller approach. That approach means ,a common controller for all pages, processes the requests.</t>
+  </si>
+  <si>
+    <t>No separation of concerns. As we discussed that every page (.aspx) has it’s own controller (code behind i.e. aspx.cs/.vb file), so both are tightly coupled.</t>
+  </si>
+  <si>
+    <t>Very clean separation of concerns. View and Controller are neatly separate.</t>
+  </si>
+  <si>
+    <t>Because of this coupled behavior, automated testing is really difficult.</t>
+  </si>
+  <si>
+    <t>In order to achieve stateful behavior, viewstate is used. Purpose was to give developers, the same experience of a typical WinForms application.</t>
+  </si>
+  <si>
+    <t>ASP.NET MVC approach is stateless as that of the web. So here no concept of viewstate.</t>
+  </si>
+  <si>
+    <t>Statefulness has a lots of problem for web environment in case of excessively large viewstate. Large viewstate means increase in page size.</t>
+  </si>
+  <si>
+    <t>As controller and view are not dependent and also no viewstate concept in ASP.NET MVC, so output is very clean.</t>
+  </si>
+  <si>
+    <t>ASP.NET WebForms model follows a Page Life cycle.</t>
+  </si>
+  <si>
+    <t>No Page Life cycle like WebForms. Request cycle is simple in ASP.NET MVC model.</t>
+  </si>
+  <si>
+    <t>Along with statefulness, microsoft tries to introduce server-side controls as in Windows applications. Purpose was to provide  somehow an abstraction to the details of HTML. In ASP.NET Web Forms, minimal knowledge of HTML, JavaScript and CSS is required.</t>
+  </si>
+  <si>
+    <t>In MVC, detailed knowledge of HTML, JavaScript and CSS is required.</t>
+  </si>
+  <si>
+    <t>Above abstraction was good but provides limited control over HTML, JavaScript and CSS which is necessary in many cases.</t>
+  </si>
+  <si>
+    <t>Full control over HTML, JavaScript and CSS.</t>
+  </si>
+  <si>
+    <t>With a lots of control libraries availability and limited knowledge of other related technologies, ASP.NET WebForms is RAD(Rapid Application Development) approach.</t>
+  </si>
+  <si>
+    <t>It’s a step back. For developers decrease in productivity.</t>
+  </si>
+  <si>
+    <t>It’s good for small scale applications with limited team size.</t>
+  </si>
+  <si>
+    <t>It’s better as well as recommended approach for large-scale applications where different teams are working together.</t>
+  </si>
+  <si>
+    <t>Testability is key feature in ASP.NET MVC. Test driven development is quite simple using this approach.</t>
+  </si>
+  <si>
+    <t> Please follow here for demo on building testable applications.</t>
+  </si>
+  <si>
+    <t>Further, if you are interested to practically learn ASP.NET MVC5, a recommended Video Series especially designed for those familiar with ASP.NET WebForms</t>
+  </si>
+  <si>
+    <t>follow here.</t>
+  </si>
+  <si>
+    <t>Curriculum here.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Inherit"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF444444"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Bookman Old Style"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -69,16 +193,99 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Bookman Old Style"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Bookman Old Style"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Bookman Old Style"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -97,6 +304,17 @@
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{EF780EE3-BBBF-4EA5-AB64-220EA636BECF}" name="Question"/>
     <tableColumn id="2" xr3:uid="{8778B80E-3141-43C9-9B88-6984136A214D}" name="Answers"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{25DD7433-C426-4802-8A00-7BA50D9BD76E}" name="Table2" displayName="Table2" ref="A2:B12" totalsRowShown="0" headerRowDxfId="3" dataDxfId="0">
+  <autoFilter ref="A2:B12" xr:uid="{26D3D1DC-B29A-400C-A32C-755D8C8C85ED}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{4495D149-C2F4-4E2A-B4EF-2376117877B9}" name="ASP.Net Web Form" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{C01F06CA-E818-44DE-AD87-3ADA5922C4B1}" name="ASP.Net MVC" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -401,17 +619,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60249798-AB4A-420E-B860-53D6A7304F32}">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="73.140625" customWidth="1"/>
-    <col min="2" max="2" width="173.7109375" customWidth="1"/>
+    <col min="1" max="1" width="84.42578125" customWidth="1"/>
+    <col min="2" max="2" width="178" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -425,4 +643,236 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16A55A76-AD96-42DD-A6CD-D71EE9D044DB}">
+  <dimension ref="A1:G31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="82.140625" customWidth="1"/>
+    <col min="2" max="2" width="73.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1"/>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="63">
+      <c r="A3" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="47.25">
+      <c r="A4" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="47.25">
+      <c r="A5" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="47.25">
+      <c r="A6" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="47.25">
+      <c r="A7" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="31.5">
+      <c r="A8" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="78.75">
+      <c r="A9" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G9" s="2"/>
+    </row>
+    <row r="10" spans="1:7" ht="47.25">
+      <c r="A10" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="G10" s="2"/>
+    </row>
+    <row r="11" spans="1:7" ht="63">
+      <c r="A11" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="G11" s="3"/>
+    </row>
+    <row r="12" spans="1:7" ht="47.25">
+      <c r="A12" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="G12" s="3"/>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="6"/>
+      <c r="B13" s="6"/>
+      <c r="G13" s="3"/>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="6"/>
+      <c r="B14" s="6"/>
+      <c r="G14" s="3"/>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="6"/>
+      <c r="B15" s="6"/>
+      <c r="G15" s="3"/>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G16" s="4"/>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="6"/>
+      <c r="B17" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G17" s="3"/>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="6"/>
+      <c r="B18" s="6"/>
+      <c r="G18" s="3"/>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="6"/>
+      <c r="B19" s="6"/>
+      <c r="G19" s="3"/>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" s="6"/>
+      <c r="B20" s="6"/>
+      <c r="G20" s="3"/>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" s="6"/>
+      <c r="B21" s="6"/>
+      <c r="G21" s="3"/>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" s="6"/>
+      <c r="B22" s="6"/>
+      <c r="G22" s="3"/>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="6"/>
+      <c r="B23" s="6"/>
+      <c r="G23" s="3"/>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="6"/>
+      <c r="B24" s="6"/>
+      <c r="G24" s="3"/>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" s="6"/>
+      <c r="B25" s="6"/>
+      <c r="G25" s="3"/>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" s="6"/>
+      <c r="B26" s="6"/>
+      <c r="G26" s="3"/>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" s="6"/>
+      <c r="B27" s="6"/>
+      <c r="G27" s="3"/>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" s="6"/>
+      <c r="B28" s="6"/>
+      <c r="G28" s="3"/>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" s="6"/>
+      <c r="B29" s="6"/>
+      <c r="G29" s="3"/>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" s="6"/>
+      <c r="B30" s="6"/>
+      <c r="G30" s="3"/>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" s="6"/>
+      <c r="B31" s="6"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="C5" r:id="rId1" display="http://msdn.microsoft.com/en-us/magazine/dd942838.aspx" xr:uid="{89672DAE-4126-4033-BD56-63BB5AE11DEC}"/>
+    <hyperlink ref="B16" r:id="rId2" display="http://click.linksynergy.com/link?id=s8waqo9RNjU&amp;offerid=323058.611518&amp;type=2&amp;murl=https%3A%2F%2Fwww.udemy.com%2Fmaruti-mvc5%2F" xr:uid="{4E952F1D-8FA7-4BAA-BABA-35934900935E}"/>
+    <hyperlink ref="B17" r:id="rId3" display="http://click.linksynergy.com/link?id=s8waqo9RNjU&amp;offerid=323058.611518&amp;type=2&amp;murl=https%3A%2F%2Fwww.udemy.com%2Fmaruti-mvc5%2F" xr:uid="{797F2A86-81A7-41A9-8D26-84202E32323B}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
+  <tableParts count="1">
+    <tablePart r:id="rId5"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>